<commit_message>
startet new mainboard PCB
</commit_message>
<xml_diff>
--- a/octanis_eps/BOM EPS octanis1.xlsx
+++ b/octanis_eps/BOM EPS octanis1.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="550" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23540" tabRatio="550"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -308,11 +312,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -320,24 +321,24 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="11"/>
+      <name val="Conakry"/>
+      <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Conakry"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -380,7 +381,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -388,73 +389,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -513,44 +473,364 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="14.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6377551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="14.4285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="35.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="14.4285714285714"/>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="2" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -576,18 +856,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="4">
         <v>6.35</v>
       </c>
-      <c r="C4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">B4*C4</f>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D13" si="0">B4*C4</f>
         <v>6.35</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -603,18 +883,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="4">
         <v>11.1</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">B5*C5</f>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
         <v>11.1</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -630,18 +910,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="4">
         <v>2.85</v>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <f aca="false">B6*C6</f>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -657,18 +937,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="4">
         <v>1.7</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <f aca="false">B7*C7</f>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -684,18 +964,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="4">
         <v>3.5</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="4">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <f aca="false">B8*C8</f>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -711,18 +991,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="4">
         <v>10.15</v>
       </c>
-      <c r="C9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <f aca="false">B9*C9</f>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
         <v>10.15</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -738,18 +1018,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="4">
         <v>3.6</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="n">
-        <f aca="false">B10*C10</f>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -765,19 +1045,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>0.038</v>
-      </c>
-      <c r="C11" s="4" t="n">
+      <c r="B11" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C11" s="4">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="n">
-        <f aca="false">B11*C11</f>
-        <v>0.114</v>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11399999999999999</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>36</v>
@@ -792,18 +1072,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="4">
         <v>1.25</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="4">
         <v>3</v>
       </c>
-      <c r="D12" s="1" t="n">
-        <f aca="false">B12*C12</f>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -819,19 +1099,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>0.713</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <f aca="false">B13*C13</f>
-        <v>0.713</v>
+      <c r="B13" s="4">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71299999999999997</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>44</v>
@@ -846,7 +1126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
         <v>2</v>
       </c>
@@ -872,24 +1152,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="C15" s="4" t="n">
+      <c r="B15" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <f aca="false">B15*C15</f>
-        <v>0.045</v>
+      <c r="D15" s="1">
+        <f t="shared" ref="D15:D50" si="1">B15*C15</f>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4">
         <v>603</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -897,24 +1177,24 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="4">
         <v>0.1</v>
       </c>
-      <c r="C16" s="4" t="n">
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <f aca="false">B16*C16</f>
-        <v>0.3</v>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="4">
         <v>1206</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -924,24 +1204,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="4" t="n">
+      <c r="B17" s="4">
         <v>0.03</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="C17" s="4">
         <v>6</v>
       </c>
-      <c r="D17" s="1" t="n">
-        <f aca="false">B17*C17</f>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="4">
         <v>603</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -949,435 +1229,435 @@
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="4" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="C18" s="4" t="n">
+      <c r="B18" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C18" s="4">
         <v>5</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <f aca="false">B18*C18</f>
-        <v>0.075</v>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="4">
         <v>603</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="4" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="C19" s="4" t="n">
+      <c r="B19" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C19" s="4">
         <v>5</v>
       </c>
-      <c r="D19" s="1" t="n">
-        <f aca="false">B19*C19</f>
-        <v>0.075</v>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="4">
         <v>603</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="4" t="n">
+      <c r="B20" s="4">
         <v>0.03</v>
       </c>
-      <c r="C20" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <f aca="false">B20*C20</f>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="4">
         <v>603</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="4">
         <v>0.03</v>
       </c>
-      <c r="C21" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <f aca="false">B21*C21</f>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="4">
         <v>603</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8">
       <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C22" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <f aca="false">B22*C22</f>
+      <c r="B22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="4">
         <v>603</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C23" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <f aca="false">B23*C23</f>
+      <c r="B23" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="4">
         <v>603</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="4">
         <v>0.1</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="4">
         <v>2</v>
       </c>
-      <c r="D24" s="1" t="n">
-        <f aca="false">B24*C24</f>
+      <c r="D24" s="1">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="4">
         <v>603</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <f aca="false">B25*C25</f>
+      <c r="B25" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="4">
         <v>603</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <f aca="false">B26*C26</f>
+      <c r="B26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="4">
         <v>603</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C27" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <f aca="false">B27*C27</f>
+      <c r="B27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="4">
         <v>603</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C28" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <f aca="false">B28*C28</f>
+      <c r="B28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="4">
         <v>603</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:8">
       <c r="A29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C29" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <f aca="false">B29*C29</f>
+      <c r="B29" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="4">
         <v>603</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="4" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="C30" s="4" t="n">
+      <c r="B30" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C30" s="4">
         <v>6</v>
       </c>
-      <c r="D30" s="1" t="n">
-        <f aca="false">B30*C30</f>
+      <c r="D30" s="1">
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="4">
         <v>603</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="4" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="C31" s="1" t="n">
+      <c r="B31" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C31" s="1">
         <v>3</v>
       </c>
-      <c r="D31" s="1" t="n">
-        <f aca="false">B31*C31</f>
-        <v>0.045</v>
-      </c>
-      <c r="F31" s="4" t="n">
+      <c r="D31" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F31" s="4">
         <v>603</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="1">
         <v>0.03</v>
       </c>
-      <c r="C32" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <f aca="false">B32*C32</f>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="4">
         <v>603</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="1">
         <v>0.03</v>
       </c>
-      <c r="C33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <f aca="false">B33*C33</f>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="4">
         <v>603</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="1">
         <v>0.03</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <f aca="false">B34*C34</f>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="4">
         <v>603</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="1">
         <v>0.03</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <f aca="false">B35*C35</f>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="F35" s="4">
         <v>603</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8">
       <c r="A36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="4" t="n">
+      <c r="B36" s="4">
         <v>0.9</v>
       </c>
-      <c r="C36" s="4" t="n">
+      <c r="C36" s="4">
         <v>3</v>
       </c>
-      <c r="D36" s="1" t="n">
-        <f aca="false">B36*C36</f>
+      <c r="D36" s="1">
+        <f t="shared" si="1"/>
         <v>2.7</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -1393,114 +1673,114 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8">
       <c r="A37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="4" t="n">
+      <c r="B37" s="4">
         <v>0.03</v>
       </c>
-      <c r="C37" s="4" t="n">
+      <c r="C37" s="4">
         <v>4</v>
       </c>
-      <c r="D37" s="1" t="n">
-        <f aca="false">B37*C37</f>
+      <c r="D37" s="1">
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="4">
         <v>603</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:8">
       <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="4" t="n">
+      <c r="B38" s="4">
         <v>0.03</v>
       </c>
-      <c r="C38" s="4" t="n">
+      <c r="C38" s="4">
         <v>10</v>
       </c>
-      <c r="D38" s="1" t="n">
-        <f aca="false">B38*C38</f>
+      <c r="D38" s="1">
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="4">
         <v>603</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:8">
       <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="4" t="n">
+      <c r="B39" s="4">
         <v>0.03</v>
       </c>
-      <c r="C39" s="4" t="n">
+      <c r="C39" s="4">
         <v>10</v>
       </c>
-      <c r="D39" s="1" t="n">
-        <f aca="false">B39*C39</f>
+      <c r="D39" s="1">
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="4">
         <v>603</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8">
       <c r="A40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C40" s="4" t="n">
+      <c r="B40" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C40" s="4">
         <v>2</v>
       </c>
-      <c r="D40" s="1" t="n">
-        <f aca="false">B40*C40</f>
+      <c r="D40" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="4">
         <v>603</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:8">
       <c r="A41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C41" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <f aca="false">B41*C41</f>
+      <c r="B41" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -1516,18 +1796,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C42" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <f aca="false">B42*C42</f>
+      <c r="B42" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -1543,72 +1823,72 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:8">
       <c r="A43" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="4" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="C43" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <f aca="false">B43*C43</f>
-        <v>0.003</v>
+      <c r="B43" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="4">
         <v>603</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="4" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="C44" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <f aca="false">B44*C44</f>
-        <v>0.003</v>
+      <c r="B44" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="4">
         <v>603</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:8">
       <c r="A45" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C45" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1" t="n">
-        <f aca="false">B45*C45</f>
+      <c r="B45" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="4" t="n">
+      <c r="F45" s="4">
         <v>1206</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -1618,24 +1898,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1">
       <c r="A46" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C46" s="4" t="n">
+      <c r="B46" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C46" s="4">
         <v>2</v>
       </c>
-      <c r="D46" s="1" t="n">
-        <f aca="false">B46*C46</f>
+      <c r="D46" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="4">
         <v>603</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -1645,24 +1925,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C47" s="4" t="n">
+      <c r="B47" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C47" s="4">
         <v>2</v>
       </c>
-      <c r="D47" s="1" t="n">
-        <f aca="false">B47*C47</f>
+      <c r="D47" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F47" s="4" t="n">
+      <c r="F47" s="4">
         <v>1206</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -1672,18 +1952,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="4" t="n">
+      <c r="B48" s="4">
         <v>1.25</v>
       </c>
-      <c r="C48" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1" t="n">
-        <f aca="false">B48*C48</f>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -1699,18 +1979,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="4" t="n">
+      <c r="B49" s="4">
         <v>1.2</v>
       </c>
-      <c r="C49" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1" t="n">
-        <f aca="false">B49*C49</f>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="E49" s="4" t="s">
@@ -1726,18 +2006,18 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C50" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" t="n">
-        <f aca="false">B50*C50</f>
+      <c r="B50" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="E50" s="4" t="s">
@@ -1753,22 +2033,22 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:8" ht="15.75" customHeight="1">
       <c r="C51" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="1" t="n">
-        <f aca="false">SUM(D15:D50,D4:D13)</f>
-        <v>78.893</v>
+      <c r="D51" s="1">
+        <f>SUM(D15:D50,D4:D13)</f>
+        <v>78.893000000000001</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>